<commit_message>
Finalize sound dataset in xlsx form
</commit_message>
<xml_diff>
--- a/dataset/final_taylor_swift_sound.xlsx
+++ b/dataset/final_taylor_swift_sound.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduard\Documents\Training\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deguedu\Downloads\dataset\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C658CC5-86EF-40FB-9965-08225BFEB1A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A6AA90-2D89-49DB-AC0F-4F71EC65EEC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FA1A5835-3FA7-4840-A3F2-F8A895CACEE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FA1A5835-3FA7-4840-A3F2-F8A895CACEE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$143</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$143</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -918,16 +918,16 @@
   <dimension ref="A1:M143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K80" sqref="K80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -968,7 +968,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>44</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>47</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>48</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>49</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>50</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>51</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>52</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>53</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>54</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>55</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>56</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>57</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>22</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>58</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>60</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>61</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>62</v>
       </c>
@@ -3059,7 +3059,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>63</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>64</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>65</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>66</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>59</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>67</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>68</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>69</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>70</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>71</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>72</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>73</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>74</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>75</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>76</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>77</v>
       </c>
@@ -3715,7 +3715,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>78</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>79</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>80</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>81</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>82</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>83</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>84</v>
       </c>
@@ -4002,7 +4002,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>85</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>86</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>87</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>88</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>89</v>
       </c>
@@ -4207,7 +4207,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>91</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>92</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>166</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>93</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>94</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>95</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>96</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>97</v>
       </c>
@@ -4535,7 +4535,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>98</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>99</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>167</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>100</v>
       </c>
@@ -4699,7 +4699,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>168</v>
       </c>
@@ -4740,7 +4740,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>169</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>101</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>102</v>
       </c>
@@ -4863,7 +4863,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>103</v>
       </c>
@@ -4904,7 +4904,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>104</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>105</v>
       </c>
@@ -4986,7 +4986,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>106</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>107</v>
       </c>
@@ -5068,7 +5068,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>108</v>
       </c>
@@ -5109,7 +5109,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>109</v>
       </c>
@@ -5150,7 +5150,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>110</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>111</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>161</v>
       </c>
@@ -5273,7 +5273,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>112</v>
       </c>
@@ -5314,7 +5314,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>113</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>114</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>162</v>
       </c>
@@ -5437,7 +5437,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>116</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>115</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>117</v>
       </c>
@@ -5560,7 +5560,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>118</v>
       </c>
@@ -5601,7 +5601,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>119</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>163</v>
       </c>
@@ -5683,7 +5683,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>120</v>
       </c>
@@ -5724,7 +5724,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>121</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>122</v>
       </c>
@@ -5806,7 +5806,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>123</v>
       </c>
@@ -5847,7 +5847,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>124</v>
       </c>
@@ -5888,7 +5888,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>125</v>
       </c>
@@ -5929,7 +5929,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>126</v>
       </c>
@@ -5970,7 +5970,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>127</v>
       </c>
@@ -6011,7 +6011,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>128</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>129</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>130</v>
       </c>
@@ -6134,7 +6134,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>131</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>133</v>
       </c>
@@ -6216,7 +6216,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>134</v>
       </c>
@@ -6257,7 +6257,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>135</v>
       </c>
@@ -6298,7 +6298,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>170</v>
       </c>
@@ -6339,7 +6339,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>136</v>
       </c>
@@ -6380,7 +6380,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>164</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>137</v>
       </c>
@@ -6462,7 +6462,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>138</v>
       </c>
@@ -6503,7 +6503,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>165</v>
       </c>
@@ -6544,7 +6544,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>139</v>
       </c>
@@ -6585,7 +6585,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>140</v>
       </c>
@@ -6626,7 +6626,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>141</v>
       </c>
@@ -6667,7 +6667,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>142</v>
       </c>
@@ -6708,7 +6708,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>143</v>
       </c>
@@ -6749,7 +6749,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>144</v>
       </c>
@@ -6791,7 +6791,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A143" xr:uid="{726582C0-4092-4D64-B6B0-7D06658330AC}"/>
+  <autoFilter ref="A1:M143" xr:uid="{AB2F6F71-82C1-41A2-8440-4B629B5F8853}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>